<commit_message>
Changed number of commodities, date validations and error messages in KPIF forms
</commit_message>
<xml_diff>
--- a/config/default/forms/app/tracking.xlsx
+++ b/config/default/forms/app/tracking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Desktop\hts\kpif release\kpif and properties\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Desktop\hts\hts_kpif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351BD22B-B72C-4AEC-A607-9AF4426F83B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41F8A3B-645F-484E-ADC2-7F5ABC83467B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47880" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -266,9 +266,6 @@
     <t>${_165004_trackingAttempted_99DCT}=”_1065_yes_99DCT”</t>
   </si>
   <si>
-    <t>Can not be more than 10</t>
-  </si>
-  <si>
     <t>_160753_dateAttempted_99DCT</t>
   </si>
   <si>
@@ -801,6 +798,9 @@
   </si>
   <si>
     <t xml:space="preserve">Informant reached </t>
+  </si>
+  <si>
+    <t>Attempt number should be between 1 and 3</t>
   </si>
 </sst>
 </file>
@@ -3780,10 +3780,10 @@
   <dimension ref="A1:Y90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D44" sqref="D44"/>
+      <selection pane="bottomRight" activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4884,7 +4884,7 @@
         <v>63</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>57</v>
@@ -4991,7 +4991,7 @@
         <v>74</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>67</v>
@@ -5001,10 +5001,10 @@
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>76</v>
+        <v>254</v>
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
@@ -5029,10 +5029,10 @@
         <v>54</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>57</v>
@@ -5045,7 +5045,7 @@
         <v>58</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
@@ -5067,13 +5067,13 @@
     </row>
     <row r="38" spans="1:25" ht="27">
       <c r="A38" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="C38" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>57</v>
@@ -5104,13 +5104,13 @@
     </row>
     <row r="39" spans="1:25" ht="27">
       <c r="A39" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="C39" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>57</v>
@@ -5141,13 +5141,13 @@
     </row>
     <row r="40" spans="1:25" ht="27">
       <c r="A40" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>57</v>
@@ -5181,14 +5181,14 @@
         <v>69</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
@@ -5213,13 +5213,13 @@
     </row>
     <row r="42" spans="1:25" ht="27">
       <c r="A42" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="C42" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>57</v>
@@ -5253,16 +5253,16 @@
         <v>69</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>67</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
@@ -5287,13 +5287,13 @@
     </row>
     <row r="44" spans="1:25" ht="27">
       <c r="A44" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>57</v>
@@ -5410,15 +5410,15 @@
         <v>13</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
@@ -5442,13 +5442,13 @@
     </row>
     <row r="50" spans="1:25" ht="27">
       <c r="A50" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="C50" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -5475,18 +5475,18 @@
     </row>
     <row r="51" spans="1:25" ht="27">
       <c r="A51" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
@@ -5510,13 +5510,13 @@
     </row>
     <row r="52" spans="1:25" ht="40.5">
       <c r="A52" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B52" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
@@ -5543,18 +5543,18 @@
     </row>
     <row r="53" spans="1:25" ht="27">
       <c r="A53" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B53" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
@@ -5578,13 +5578,13 @@
     </row>
     <row r="54" spans="1:25" ht="13.5">
       <c r="A54" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B54" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -5611,20 +5611,20 @@
     </row>
     <row r="55" spans="1:25" ht="27">
       <c r="A55" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F55" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
@@ -5648,20 +5648,20 @@
     </row>
     <row r="56" spans="1:25" ht="17.45" customHeight="1">
       <c r="A56" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
@@ -5685,13 +5685,13 @@
     </row>
     <row r="57" spans="1:25" ht="27">
       <c r="A57" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B57" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="s">
@@ -5720,18 +5720,18 @@
     </row>
     <row r="58" spans="1:25" ht="13.5">
       <c r="A58" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B58" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>121</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
@@ -5755,13 +5755,13 @@
     </row>
     <row r="59" spans="1:25" ht="27">
       <c r="A59" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B59" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5" t="s">
@@ -5790,20 +5790,20 @@
     </row>
     <row r="60" spans="1:25" ht="27">
       <c r="A60" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B60" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>125</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
@@ -5827,20 +5827,20 @@
     </row>
     <row r="61" spans="1:25" ht="27">
       <c r="A61" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B61" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>128</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
@@ -5864,20 +5864,20 @@
     </row>
     <row r="62" spans="1:25" ht="40.5">
       <c r="A62" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B62" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
@@ -5901,20 +5901,20 @@
     </row>
     <row r="63" spans="1:25" ht="40.5">
       <c r="A63" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B63" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C63" s="11" t="s">
         <v>133</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>134</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
@@ -5938,20 +5938,20 @@
     </row>
     <row r="64" spans="1:25" ht="27">
       <c r="A64" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B64" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="11" t="s">
         <v>136</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>137</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
@@ -6002,13 +6002,13 @@
     </row>
     <row r="66" spans="1:25" ht="27">
       <c r="A66" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B66" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="s">
@@ -6037,18 +6037,18 @@
     </row>
     <row r="67" spans="1:25" ht="13.5">
       <c r="A67" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B67" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C67" s="10" t="s">
         <v>141</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>142</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
       <c r="F67" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
@@ -6099,13 +6099,13 @@
     </row>
     <row r="69" spans="1:25" ht="13.5">
       <c r="A69" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B69" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
@@ -6132,20 +6132,20 @@
     </row>
     <row r="70" spans="1:25" ht="27">
       <c r="A70" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B70" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
@@ -6169,20 +6169,20 @@
     </row>
     <row r="71" spans="1:25" ht="27">
       <c r="A71" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B71" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" s="10" t="s">
         <v>147</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>148</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
@@ -6206,13 +6206,13 @@
     </row>
     <row r="72" spans="1:25" ht="13.5">
       <c r="A72" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B72" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
@@ -6239,20 +6239,20 @@
     </row>
     <row r="73" spans="1:25" ht="27">
       <c r="A73" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B73" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>153</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
@@ -6276,20 +6276,20 @@
     </row>
     <row r="74" spans="1:25" ht="54">
       <c r="A74" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B74" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74" s="10" t="s">
         <v>155</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>156</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
@@ -6313,20 +6313,20 @@
     </row>
     <row r="75" spans="1:25" ht="27">
       <c r="A75" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B75" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C75" s="10" t="s">
         <v>158</v>
-      </c>
-      <c r="C75" s="10" t="s">
-        <v>159</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
@@ -6350,13 +6350,13 @@
     </row>
     <row r="76" spans="1:25" ht="27">
       <c r="A76" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B76" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>162</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="4" t="s">
@@ -6385,20 +6385,20 @@
     </row>
     <row r="77" spans="1:25" ht="27">
       <c r="A77" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B77" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C77" s="11" t="s">
         <v>163</v>
-      </c>
-      <c r="C77" s="11" t="s">
-        <v>164</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
@@ -6422,20 +6422,20 @@
     </row>
     <row r="78" spans="1:25" ht="27">
       <c r="A78" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B78" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C78" s="11" t="s">
         <v>166</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>167</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
@@ -6459,20 +6459,20 @@
     </row>
     <row r="79" spans="1:25" ht="27">
       <c r="A79" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B79" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C79" s="11" t="s">
         <v>169</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>170</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G79" s="5"/>
       <c r="H79" s="5"/>
@@ -6496,20 +6496,20 @@
     </row>
     <row r="80" spans="1:25" ht="27">
       <c r="A80" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B80" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C80" s="11" t="s">
         <v>172</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>173</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
@@ -6533,20 +6533,20 @@
     </row>
     <row r="81" spans="1:25" ht="27">
       <c r="A81" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B81" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" s="11" t="s">
         <v>175</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>176</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
@@ -6570,20 +6570,20 @@
     </row>
     <row r="82" spans="1:25" ht="27">
       <c r="A82" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B82" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C82" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>179</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
@@ -6607,20 +6607,20 @@
     </row>
     <row r="83" spans="1:25" ht="27">
       <c r="A83" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B83" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C83" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="C83" s="11" t="s">
-        <v>182</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
@@ -6644,20 +6644,20 @@
     </row>
     <row r="84" spans="1:25" ht="27">
       <c r="A84" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B84" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C84" s="11" t="s">
         <v>184</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>185</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
@@ -6681,13 +6681,13 @@
     </row>
     <row r="85" spans="1:25" ht="27">
       <c r="A85" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B85" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C85" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>188</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="4" t="s">
@@ -6716,20 +6716,20 @@
     </row>
     <row r="86" spans="1:25" ht="40.5">
       <c r="A86" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B86" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C86" s="11" t="s">
         <v>189</v>
-      </c>
-      <c r="C86" s="11" t="s">
-        <v>190</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
@@ -6753,20 +6753,20 @@
     </row>
     <row r="87" spans="1:25" ht="40.5">
       <c r="A87" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B87" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="C87" s="11" t="s">
         <v>192</v>
-      </c>
-      <c r="C87" s="11" t="s">
-        <v>193</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G87" s="5"/>
       <c r="H87" s="5"/>
@@ -6788,22 +6788,22 @@
       <c r="X87" s="5"/>
       <c r="Y87" s="5"/>
     </row>
-    <row r="88" spans="1:25" ht="40.5">
+    <row r="88" spans="1:25" ht="27">
       <c r="A88" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B88" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C88" s="11" t="s">
         <v>195</v>
-      </c>
-      <c r="C88" s="11" t="s">
-        <v>196</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G88" s="5"/>
       <c r="H88" s="5"/>
@@ -6827,20 +6827,20 @@
     </row>
     <row r="89" spans="1:25" ht="27">
       <c r="A89" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
@@ -8198,7 +8198,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13.9">
       <c r="A1" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
@@ -8212,299 +8212,299 @@
     </row>
     <row r="2" spans="1:6" ht="13.5">
       <c r="A2" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>202</v>
-      </c>
       <c r="C2" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>205</v>
-      </c>
       <c r="C4" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>211</v>
-      </c>
       <c r="C9" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="C11" s="11" t="s">
         <v>214</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>219</v>
-      </c>
       <c r="C14" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>228</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B23" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>232</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>233</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>235</v>
-      </c>
       <c r="C25" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="1048543" ht="15.75" customHeight="1"/>
@@ -8530,42 +8530,42 @@
     <col min="4" max="1025" width="14.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.75">
+    <row r="1" spans="1:6" ht="13.9">
       <c r="A1" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>242</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="27">
       <c r="A2" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" s="15">
         <f ca="1">NOW()</f>
-        <v>44091.534743634256</v>
+        <v>44102.640432291664</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>244</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>245</v>
       </c>
       <c r="F2" s="10"/>
     </row>

</xml_diff>